<commit_message>
Update unit tests to include checksum and duplicate testing
</commit_message>
<xml_diff>
--- a/test/some_files.xlsx
+++ b/test/some_files.xlsx
@@ -14,78 +14,105 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="33">
+  <si>
+    <t>File Path</t>
+  </si>
+  <si>
+    <t>Filename</t>
+  </si>
+  <si>
+    <t>Extension</t>
+  </si>
+  <si>
+    <t>File Size</t>
+  </si>
+  <si>
+    <t>File Size (bytes)</t>
+  </si>
+  <si>
+    <t>Duplicate</t>
+  </si>
   <si>
     <t>Directory</t>
   </si>
   <si>
-    <t>Extension</t>
-  </si>
-  <si>
-    <t>File Path</t>
-  </si>
-  <si>
-    <t>File Size</t>
-  </si>
-  <si>
-    <t>File Size (bytes)</t>
-  </si>
-  <si>
-    <t>Filename</t>
+    <t>Checksum</t>
+  </si>
+  <si>
+    <t>c:\Users\cdevore\Documents\GitHub\DocumentCatalog\test\Email Security Digest 5 New Messages .msg</t>
+  </si>
+  <si>
+    <t>c:\Users\cdevore\Documents\GitHub\DocumentCatalog\test\email02.msg</t>
+  </si>
+  <si>
+    <t>c:\Users\cdevore\Documents\GitHub\DocumentCatalog\test\some_files.xlsx</t>
+  </si>
+  <si>
+    <t>c:\Users\cdevore\Documents\GitHub\DocumentCatalog\test\text1.txt</t>
+  </si>
+  <si>
+    <t>c:\Users\cdevore\Documents\GitHub\DocumentCatalog\test\this is an Excel spreadsheet.xlsx</t>
+  </si>
+  <si>
+    <t>c:\Users\cdevore\Documents\GitHub\DocumentCatalog\test\this_is_a_word_document.docx</t>
+  </si>
+  <si>
+    <t>Email Security Digest 5 New Messages .msg</t>
+  </si>
+  <si>
+    <t>email02.msg</t>
+  </si>
+  <si>
+    <t>some_files.xlsx</t>
+  </si>
+  <si>
+    <t>text1.txt</t>
+  </si>
+  <si>
+    <t>this is an Excel spreadsheet.xlsx</t>
+  </si>
+  <si>
+    <t>this_is_a_word_document.docx</t>
+  </si>
+  <si>
+    <t>.msg</t>
+  </si>
+  <si>
+    <t>.xlsx</t>
+  </si>
+  <si>
+    <t>.txt</t>
+  </si>
+  <si>
+    <t>.docx</t>
+  </si>
+  <si>
+    <t>64KB</t>
+  </si>
+  <si>
+    <t>6KB</t>
+  </si>
+  <si>
+    <t>0B</t>
   </si>
   <si>
     <t>c:\Users\cdevore\Documents\GitHub\DocumentCatalog\test</t>
   </si>
   <si>
-    <t>.msg</t>
-  </si>
-  <si>
-    <t>.txt</t>
-  </si>
-  <si>
-    <t>.xlsx</t>
-  </si>
-  <si>
-    <t>.docx</t>
-  </si>
-  <si>
-    <t>c:\Users\cdevore\Documents\GitHub\DocumentCatalog\test\Email Security Digest 5 New Messages .msg</t>
-  </si>
-  <si>
-    <t>c:\Users\cdevore\Documents\GitHub\DocumentCatalog\test\email02.msg</t>
-  </si>
-  <si>
-    <t>c:\Users\cdevore\Documents\GitHub\DocumentCatalog\test\text1.txt</t>
-  </si>
-  <si>
-    <t>c:\Users\cdevore\Documents\GitHub\DocumentCatalog\test\this is an Excel spreadsheet.xlsx</t>
-  </si>
-  <si>
-    <t>c:\Users\cdevore\Documents\GitHub\DocumentCatalog\test\this_is_a_word_document.docx</t>
-  </si>
-  <si>
-    <t>64KB</t>
-  </si>
-  <si>
-    <t>0B</t>
-  </si>
-  <si>
-    <t>6KB</t>
-  </si>
-  <si>
-    <t>Email Security Digest 5 New Messages .msg</t>
-  </si>
-  <si>
-    <t>email02.msg</t>
-  </si>
-  <si>
-    <t>text1.txt</t>
-  </si>
-  <si>
-    <t>this is an Excel spreadsheet.xlsx</t>
-  </si>
-  <si>
-    <t>this_is_a_word_document.docx</t>
+    <t>b8b8f59c500d3ce9e6392e1c1b2ffc53af78e838</t>
+  </si>
+  <si>
+    <t>daa063c933cbdfd82dae57b451dcc488c8c19a0f</t>
+  </si>
+  <si>
+    <t>caa4bafef00ef9915deafb1344beca6c34640538</t>
+  </si>
+  <si>
+    <t>da39a3ee5e6b4b0d3255bfef95601890afd80709</t>
+  </si>
+  <si>
+    <t>edf0ec1ae0430ed567294e292a69dd371a4de939</t>
   </si>
 </sst>
 </file>
@@ -443,13 +470,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:9">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -468,120 +495,185 @@
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:9">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="F2">
         <v>65024</v>
       </c>
-      <c r="G2" t="s">
-        <v>19</v>
+      <c r="G2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:9">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="F3">
         <v>66048</v>
       </c>
-      <c r="G3" t="s">
-        <v>20</v>
+      <c r="G3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" t="s">
+        <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:9">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4" t="s">
-        <v>21</v>
+        <v>5804</v>
+      </c>
+      <c r="G4" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" t="s">
+        <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:9">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="F5">
-        <v>6171</v>
-      </c>
-      <c r="G5" t="s">
-        <v>22</v>
+        <v>0</v>
+      </c>
+      <c r="G5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" t="s">
+        <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:9">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E6" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6" t="s">
+        <v>6171</v>
+      </c>
+      <c r="G6" t="b">
+        <v>0</v>
+      </c>
+      <c r="H6" t="s">
+        <v>27</v>
+      </c>
+      <c r="I6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
         <v>23</v>
+      </c>
+      <c r="E7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7" t="b">
+        <v>1</v>
+      </c>
+      <c r="H7" t="s">
+        <v>27</v>
+      </c>
+      <c r="I7" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update unit tests for existing catalog
</commit_message>
<xml_diff>
--- a/test/some_files.xlsx
+++ b/test/some_files.xlsx
@@ -7,18 +7,25 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Catalog" sheetId="1" r:id="rId1"/>
+    <sheet name="Properties" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="45">
   <si>
     <t>File Path</t>
   </si>
   <si>
+    <t>Base Directory</t>
+  </si>
+  <si>
+    <t>Relative Path</t>
+  </si>
+  <si>
     <t>Filename</t>
   </si>
   <si>
@@ -28,34 +35,46 @@
     <t>File Size</t>
   </si>
   <si>
-    <t>File Size (bytes)</t>
+    <t>Readable Size</t>
+  </si>
+  <si>
+    <t>Checksum</t>
   </si>
   <si>
     <t>Duplicate</t>
   </si>
   <si>
+    <t>File Link</t>
+  </si>
+  <si>
     <t>Directory</t>
   </si>
   <si>
-    <t>Checksum</t>
-  </si>
-  <si>
-    <t>c:\Users\cdevore\Documents\GitHub\DocumentCatalog\test\Email Security Digest 5 New Messages .msg</t>
-  </si>
-  <si>
-    <t>c:\Users\cdevore\Documents\GitHub\DocumentCatalog\test\email02.msg</t>
-  </si>
-  <si>
-    <t>c:\Users\cdevore\Documents\GitHub\DocumentCatalog\test\some_files.xlsx</t>
-  </si>
-  <si>
-    <t>c:\Users\cdevore\Documents\GitHub\DocumentCatalog\test\text1.txt</t>
-  </si>
-  <si>
-    <t>c:\Users\cdevore\Documents\GitHub\DocumentCatalog\test\this is an Excel spreadsheet.xlsx</t>
-  </si>
-  <si>
-    <t>c:\Users\cdevore\Documents\GitHub\DocumentCatalog\test\this_is_a_word_document.docx</t>
+    <t>Link Directory</t>
+  </si>
+  <si>
+    <t>Link Name</t>
+  </si>
+  <si>
+    <t>C:\Users\cdevore\Documents\GitHub\DocumentCatalog\test\Email Security Digest 5 New Messages .msg</t>
+  </si>
+  <si>
+    <t>C:\Users\cdevore\Documents\GitHub\DocumentCatalog\test\email02.msg</t>
+  </si>
+  <si>
+    <t>C:\Users\cdevore\Documents\GitHub\DocumentCatalog\test\some_files.xlsx</t>
+  </si>
+  <si>
+    <t>C:\Users\cdevore\Documents\GitHub\DocumentCatalog\test\text1.txt</t>
+  </si>
+  <si>
+    <t>C:\Users\cdevore\Documents\GitHub\DocumentCatalog\test\this is an Excel spreadsheet.xlsx</t>
+  </si>
+  <si>
+    <t>C:\Users\cdevore\Documents\GitHub\DocumentCatalog\test\this_is_a_word_document.docx</t>
+  </si>
+  <si>
+    <t>C:\Users\cdevore\Documents\GitHub\DocumentCatalog\test</t>
   </si>
   <si>
     <t>Email Security Digest 5 New Messages .msg</t>
@@ -97,22 +116,40 @@
     <t>0B</t>
   </si>
   <si>
-    <t>c:\Users\cdevore\Documents\GitHub\DocumentCatalog\test</t>
-  </si>
-  <si>
     <t>b8b8f59c500d3ce9e6392e1c1b2ffc53af78e838</t>
   </si>
   <si>
     <t>daa063c933cbdfd82dae57b451dcc488c8c19a0f</t>
   </si>
   <si>
-    <t>caa4bafef00ef9915deafb1344beca6c34640538</t>
+    <t>187654a5831d5fec4c497a59f78d4c13aae7fffc</t>
   </si>
   <si>
     <t>da39a3ee5e6b4b0d3255bfef95601890afd80709</t>
   </si>
   <si>
     <t>edf0ec1ae0430ed567294e292a69dd371a4de939</t>
+  </si>
+  <si>
+    <t>Document Catalog Properties</t>
+  </si>
+  <si>
+    <t>Search Directories:</t>
+  </si>
+  <si>
+    <t>Exclude Directories:</t>
+  </si>
+  <si>
+    <t>sub_dir</t>
+  </si>
+  <si>
+    <t>Buffer Size:</t>
+  </si>
+  <si>
+    <t>Hash Function:</t>
+  </si>
+  <si>
+    <t>sha1</t>
   </si>
 </sst>
 </file>
@@ -470,13 +507,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:14">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -501,179 +538,262 @@
       <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
         <v>20</v>
       </c>
       <c r="E2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2">
+        <v>20</v>
+      </c>
+      <c r="F2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2">
         <v>65024</v>
       </c>
-      <c r="G2" t="b">
+      <c r="H2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" t="b">
         <v>0</v>
       </c>
-      <c r="H2" t="s">
-        <v>27</v>
-      </c>
-      <c r="I2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3">
+        <v>21</v>
+      </c>
+      <c r="F3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3">
         <v>66048</v>
       </c>
-      <c r="G3" t="b">
+      <c r="H3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" t="b">
         <v>0</v>
       </c>
-      <c r="H3" t="s">
-        <v>27</v>
-      </c>
-      <c r="I3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4">
-        <v>5804</v>
-      </c>
-      <c r="G4" t="b">
+        <v>22</v>
+      </c>
+      <c r="F4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4">
+        <v>6085</v>
+      </c>
+      <c r="H4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" t="b">
         <v>0</v>
       </c>
-      <c r="H4" t="s">
-        <v>27</v>
-      </c>
-      <c r="I4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5">
+        <v>23</v>
+      </c>
+      <c r="F5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5">
         <v>0</v>
       </c>
-      <c r="G5" t="b">
+      <c r="H5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" t="s">
+        <v>36</v>
+      </c>
+      <c r="J5" t="b">
         <v>0</v>
       </c>
-      <c r="H5" t="s">
-        <v>27</v>
-      </c>
-      <c r="I5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6">
+        <v>24</v>
+      </c>
+      <c r="F6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6">
         <v>6171</v>
       </c>
-      <c r="G6" t="b">
+      <c r="H6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" t="s">
+        <v>37</v>
+      </c>
+      <c r="J6" t="b">
         <v>0</v>
       </c>
-      <c r="H6" t="s">
-        <v>27</v>
-      </c>
-      <c r="I6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
         <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E7" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7">
+        <v>25</v>
+      </c>
+      <c r="F7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7">
         <v>0</v>
       </c>
-      <c r="G7" t="b">
+      <c r="H7" t="s">
+        <v>32</v>
+      </c>
+      <c r="I7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J7" t="b">
         <v>1</v>
       </c>
-      <c r="H7" t="s">
-        <v>27</v>
-      </c>
-      <c r="I7" t="s">
-        <v>31</v>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5">
+        <v>65536</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>